<commit_message>
Añadir configuracion de colegios electorales
</commit_message>
<xml_diff>
--- a/src/main/test/resourceselecciones.xlsx
+++ b/src/main/test/resourceselecciones.xlsx
@@ -1,82 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciofernandezalvarez/Documents/asw/VotingSystem_2b/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15030" windowHeight="4125"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Inicial</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>Podemos</t>
-  </si>
-  <si>
-    <t>Partido politico</t>
-  </si>
-  <si>
-    <t>Ciudadanos</t>
-  </si>
-  <si>
-    <t>Partido Popular</t>
-  </si>
-  <si>
-    <t>PP</t>
-  </si>
-  <si>
-    <t>Cs</t>
-  </si>
-  <si>
-    <t>Partido Politico</t>
-  </si>
-  <si>
-    <t>Partido Socialista Obrero Español</t>
-  </si>
-  <si>
-    <t>PSOE</t>
-  </si>
-  <si>
-    <t>Unión Progreso y Democracia</t>
-  </si>
-  <si>
-    <t>UpyD</t>
-  </si>
-  <si>
-    <t>Izquierda Unida</t>
-  </si>
-  <si>
-    <t>IU</t>
-  </si>
-  <si>
-    <t>Vox</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Constitutency</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Polling Place</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Extremadura</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Asturias</t>
   </si>
 </sst>
 </file>
@@ -171,12 +138,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -206,12 +173,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -415,105 +382,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C5" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
+      <c r="C5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -527,7 +449,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -539,7 +461,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
posiblidad de votar en listas abiertas
</commit_message>
<xml_diff>
--- a/src/main/test/resourceselecciones.xlsx
+++ b/src/main/test/resourceselecciones.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15030" windowHeight="3690"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15030" windowHeight="4125"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,54 +17,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Partido</t>
-  </si>
-  <si>
-    <t>NIF</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>BB</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>11111111A</t>
-  </si>
-  <si>
-    <t>22222222B</t>
-  </si>
-  <si>
-    <t>33333333C</t>
-  </si>
-  <si>
-    <t>Alberto</t>
-  </si>
-  <si>
-    <t>Borja</t>
-  </si>
-  <si>
-    <t>Carlos</t>
-  </si>
-  <si>
-    <t>Apellido</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Alvarez</t>
-  </si>
-  <si>
-    <t>Baston</t>
-  </si>
-  <si>
-    <t>Cienfuegos</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Constitutency</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Polling Place</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Extremadura</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Asturias</t>
   </si>
 </sst>
 </file>
@@ -403,69 +382,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C5" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Carga de votos presenciales
</commit_message>
<xml_diff>
--- a/src/main/test/resourceselecciones.xlsx
+++ b/src/main/test/resourceselecciones.xlsx
@@ -1,49 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaciofernandezalvarez/Documents/asw/VotingSystem_2b/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15030" windowHeight="4125"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Constitutency</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Polling Place</t>
-  </si>
-  <si>
-    <t>Madrid</t>
-  </si>
-  <si>
-    <t>Extremadura</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Asturias</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Inicial</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Podemos</t>
+  </si>
+  <si>
+    <t>Partido politico</t>
+  </si>
+  <si>
+    <t>Ciudadanos</t>
+  </si>
+  <si>
+    <t>Partido Popular</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>Cs</t>
+  </si>
+  <si>
+    <t>Partido Politico</t>
+  </si>
+  <si>
+    <t>Partido Socialista Obrero Español</t>
+  </si>
+  <si>
+    <t>PSOE</t>
+  </si>
+  <si>
+    <t>Unión Progreso y Democracia</t>
+  </si>
+  <si>
+    <t>UpyD</t>
+  </si>
+  <si>
+    <t>Izquierda Unida</t>
+  </si>
+  <si>
+    <t>IU</t>
+  </si>
+  <si>
+    <t>Vox</t>
   </si>
 </sst>
 </file>
@@ -138,12 +171,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -173,12 +206,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -382,60 +415,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C3:C5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>3</v>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -449,7 +527,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -461,7 +539,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>